<commit_message>
Added Solution for Longest Consecutive Sequence
</commit_message>
<xml_diff>
--- a/DSA Important Questions.xlsx
+++ b/DSA Important Questions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="350">
   <si>
     <t>DSA Important Questions - TopicWise Mastery Plan</t>
   </si>
@@ -1482,7 +1482,7 @@
   <dimension ref="A1:Z1065"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1658,6 +1658,9 @@
       <c r="E11" s="13" t="s">
         <v>17</v>
       </c>
+      <c r="F11" s="2" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="13.2">
       <c r="A12" s="2"/>
@@ -1672,6 +1675,9 @@
       </c>
       <c r="E12" s="13" t="s">
         <v>20</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.2">

</xml_diff>

<commit_message>
Added Solution for Two Sum II
</commit_message>
<xml_diff>
--- a/DSA Important Questions.xlsx
+++ b/DSA Important Questions.xlsx
@@ -13,11 +13,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DSA Important Questions - Topic'!$A$1</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="351">
   <si>
     <t>DSA Important Questions - TopicWise Mastery Plan</t>
   </si>
@@ -1067,13 +1068,16 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1142,6 +1146,12 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1228,10 +1238,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1269,8 +1283,10 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1481,8 +1497,8 @@
   </sheetPr>
   <dimension ref="A1:Z1065"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1637,7 +1653,7 @@
       <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1694,6 +1710,9 @@
       <c r="E13" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="F13" s="2" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="13.2">
       <c r="A14" s="2"/>
@@ -1706,8 +1725,11 @@
       <c r="D14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="35" t="s">
         <v>26</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="13.2">
@@ -1721,8 +1743,11 @@
       <c r="D15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="35" t="s">
         <v>29</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.2">
@@ -1736,8 +1761,11 @@
       <c r="D16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="35" t="s">
         <v>32</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="13.2">
@@ -1805,6 +1833,9 @@
       <c r="E21" s="18" t="s">
         <v>36</v>
       </c>
+      <c r="F21" s="34" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="22" spans="1:26" ht="13.2">
       <c r="A22" s="17"/>
@@ -1820,6 +1851,9 @@
       <c r="E22" s="18" t="s">
         <v>39</v>
       </c>
+      <c r="F22" s="34" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="23" spans="1:26" ht="13.2">
       <c r="A23" s="17"/>
@@ -1834,6 +1868,9 @@
       </c>
       <c r="E23" s="18" t="s">
         <v>42</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="13.2">

</xml_diff>